<commit_message>
added generation of plots
</commit_message>
<xml_diff>
--- a/evaluation/results/results.xlsx
+++ b/evaluation/results/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2b36d7a34a6ebe0c/Dokumente/TUHH/9.3.Mastersemester/Projektarbeit/Code/paper_camera_comparison/evaluation/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0325C264-EEC8-49F8-B595-7279CC241F1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:40009_{0325C264-EEC8-49F8-B595-7279CC241F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{308EC8D1-EA81-4B40-A7D1-C9B8981A6731}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,22 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">results!$A$1:$G$85</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">setup_1_bright!$A$1:$K$31</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="80">
   <si>
     <t>camera</t>
   </si>
@@ -265,12 +275,15 @@
   </si>
   <si>
     <t>5 meter</t>
+  </si>
+  <si>
+    <t>Opt sphere pos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -753,48 +766,48 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -812,7 +825,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1569,7 +1582,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3518,7 +3531,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3813,14 +3826,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70:E70"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -3902,25 +3915,25 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>9.9045562049620103E-2</v>
+        <v>0.39691971715540703</v>
       </c>
       <c r="E3">
-        <v>7.6727961023976795E-4</v>
+        <v>1.10822482015257</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>5.6265905161528395E-4</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="K3" t="s">
         <v>62</v>
@@ -3934,25 +3947,25 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>6.8118664365912802E-3</v>
+        <v>0.39054249500646199</v>
       </c>
       <c r="E4">
-        <v>4.8283062270565403E-3</v>
+        <v>0.69093597690780295</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>4.8583790534814203E-4</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="K4" t="s">
         <v>63</v>
@@ -3966,74 +3979,77 @@
       <c r="N4" t="s">
         <v>68</v>
       </c>
+      <c r="O4" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>1.0587518011335E-2</v>
+        <v>0.38994069471942799</v>
       </c>
       <c r="E5">
-        <v>8.2919013696786201E-3</v>
-      </c>
-      <c r="F5">
-        <v>2.1615585531971101E-3</v>
+        <v>0.290810346140363</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2.8189202102245499E-5</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6">
-        <v>1.6435212053167499E-2</v>
+        <v>0.583126044419779</v>
       </c>
       <c r="E6">
-        <v>7.1600894317287202E-3</v>
+        <v>0.70275114627101298</v>
       </c>
       <c r="F6">
-        <v>7.5788442548485203E-3</v>
+        <v>1.5762807280915699E-4</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>1.7977434108671801E-2</v>
+        <v>0.56464335766478502</v>
       </c>
       <c r="E7">
-        <v>1.8647753703395401E-2</v>
+        <v>1.44037071897738</v>
       </c>
       <c r="F7">
-        <v>1.5082738977944101E-3</v>
+        <v>3.8215125201546299E-3</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -4041,137 +4057,119 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8">
-        <v>0.39691971715540703</v>
+        <v>3.3551311292107799</v>
       </c>
       <c r="E8">
-        <v>1.10822482015257</v>
+        <v>1.4290055912144</v>
       </c>
       <c r="F8">
-        <v>5.6265905161528395E-4</v>
-      </c>
-      <c r="G8" t="s">
-        <v>14</v>
+        <v>2958.6010430657702</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
       <c r="C9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>0.24588505155180099</v>
+        <v>1.6353867628952901</v>
       </c>
       <c r="E9">
-        <v>2.0987249605020401E-2</v>
+        <v>0.72960658629280795</v>
       </c>
       <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>24</v>
+        <v>11.5798418384553</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>3.5928971402492899E-3</v>
+        <v>1.4431938998148399</v>
       </c>
       <c r="E10">
-        <v>9.1002532901090106E-3</v>
+        <v>0.41701373301734701</v>
       </c>
       <c r="F10">
-        <v>6.2723467862481298E-3</v>
-      </c>
-      <c r="G10" t="s">
-        <v>30</v>
+        <v>92.637575278335405</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>3.0550116101209099E-2</v>
+        <v>1.56569575936312</v>
       </c>
       <c r="E11">
-        <v>4.55405009888704E-2</v>
+        <v>0.63742375503896198</v>
       </c>
       <c r="F11">
-        <v>4.5264828407062E-3</v>
-      </c>
-      <c r="G11" t="s">
-        <v>37</v>
+        <v>2604.4148449139602</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>3.6438361299231401E-3</v>
+        <v>1.31005315718724</v>
       </c>
       <c r="E12">
-        <v>2.2271907976498199E-2</v>
-      </c>
-      <c r="F12">
-        <v>5.79054916985951E-3</v>
+        <v>1.2056962269094</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4.8176855683120603E-6</v>
       </c>
       <c r="G12" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
         <v>2</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
       <c r="D13">
-        <v>2.7812285502499499E-2</v>
+        <v>0.99978597990104101</v>
       </c>
       <c r="E13">
-        <v>1.9913199960123799E-2</v>
-      </c>
-      <c r="F13" s="1">
-        <v>8.61821315713875E-7</v>
-      </c>
-      <c r="G13" t="s">
-        <v>49</v>
+        <v>572.24332754043496</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -4179,96 +4177,84 @@
         <v>7</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14">
-        <v>0.39054249500646199</v>
+        <v>0.99958593898769799</v>
       </c>
       <c r="E14">
-        <v>0.69093597690780295</v>
-      </c>
-      <c r="F14">
-        <v>4.8583790534814203E-4</v>
-      </c>
-      <c r="G14" t="s">
-        <v>17</v>
+        <v>710.31946600416597</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15">
-        <v>0.46016825521808702</v>
+        <v>0.99999944308530697</v>
       </c>
       <c r="E15">
-        <v>8.3064419703406597E-2</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15" t="s">
-        <v>25</v>
+        <v>145.938586744144</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>9.8694983153751296E-3</v>
+        <v>9.9045562049620103E-2</v>
       </c>
       <c r="E16">
-        <v>2.3443665060524199E-2</v>
+        <v>7.6727961023976795E-4</v>
       </c>
       <c r="F16">
-        <v>2.6343263742278501E-2</v>
+        <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>0.11265892621963999</v>
+        <v>0.24588505155180099</v>
       </c>
       <c r="E17">
-        <v>0.108580538600536</v>
+        <v>2.0987249605020401E-2</v>
       </c>
       <c r="F17">
-        <v>1.8662441527086099E-2</v>
+        <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -4277,62 +4263,62 @@
         <v>1</v>
       </c>
       <c r="D18">
-        <v>3.15363396795416E-2</v>
+        <v>0.46016825521808702</v>
       </c>
       <c r="E18">
-        <v>4.67932663299108E-2</v>
+        <v>8.3064419703406597E-2</v>
       </c>
       <c r="F18">
-        <v>4.5415234822451297E-3</v>
+        <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19">
-        <v>2.6055156398218999E-2</v>
+        <v>0.70745540120434203</v>
       </c>
       <c r="E19">
-        <v>2.4400456291021701E-2</v>
-      </c>
-      <c r="F19">
-        <v>1.1706156009953399E-3</v>
+        <v>0.177801371161392</v>
+      </c>
+      <c r="F19" s="1">
+        <v>4.37158469945355E-5</v>
       </c>
       <c r="G19" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20">
-        <v>0.38994069471942799</v>
+        <v>1.43045026948951</v>
       </c>
       <c r="E20">
-        <v>0.290810346140363</v>
-      </c>
-      <c r="F20" s="1">
-        <v>2.8189202102245499E-5</v>
+        <v>1.6520611992515899</v>
+      </c>
+      <c r="F20">
+        <v>1.9979843789367599E-4</v>
       </c>
       <c r="G20" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -4340,137 +4326,125 @@
         <v>8</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>0.70745540120434203</v>
+        <v>0.30062668071299098</v>
       </c>
       <c r="E21">
-        <v>0.177801371161392</v>
+        <v>0.232858912244334</v>
       </c>
       <c r="F21" s="1">
-        <v>4.37158469945355E-5</v>
+        <v>1.5795448936275199E-6</v>
       </c>
       <c r="G21" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D22">
-        <v>2.11816620144437E-2</v>
+        <v>3.73604017574681</v>
       </c>
       <c r="E22">
-        <v>4.2650203333278902E-2</v>
+        <v>1.74830314749601</v>
       </c>
       <c r="F22">
-        <v>2.16337438355787E-3</v>
-      </c>
-      <c r="G22" t="s">
-        <v>32</v>
+        <v>2400.21863787146</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D23">
-        <v>0.23598936342653201</v>
+        <v>1.7839608746771101</v>
       </c>
       <c r="E23">
-        <v>0.24610894859351301</v>
+        <v>0.85988434003665404</v>
       </c>
       <c r="F23">
-        <v>3.8315761234071002E-2</v>
-      </c>
-      <c r="G23" t="s">
-        <v>39</v>
+        <v>722.21443075240495</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>7.9863795705357205E-2</v>
-      </c>
-      <c r="E24">
-        <v>8.7966792709945105E-2</v>
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
       </c>
       <c r="F24">
-        <v>1.12795535261288E-2</v>
-      </c>
-      <c r="G24" t="s">
-        <v>46</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D25">
-        <v>1.5277419708914599E-2</v>
+        <v>1.7787607912916501</v>
       </c>
       <c r="E25">
-        <v>4.8098007247903099E-2</v>
+        <v>0.89380641613968603</v>
       </c>
       <c r="F25">
-        <v>1.6403662575491899E-4</v>
-      </c>
-      <c r="G25" t="s">
-        <v>53</v>
+        <v>9.3435874212267596</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26">
-        <v>0.583126044419779</v>
+        <v>0.62275282626455197</v>
       </c>
       <c r="E26">
-        <v>0.70275114627101298</v>
+        <v>0.89833380224297898</v>
       </c>
       <c r="F26">
-        <v>1.5762807280915699E-4</v>
+        <v>2.3133224739621898E-3</v>
       </c>
       <c r="G26" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -4478,160 +4452,142 @@
         <v>8</v>
       </c>
       <c r="B27">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>1.43045026948951</v>
+        <v>0.99999974794416902</v>
       </c>
       <c r="E27">
-        <v>1.6520611992515899</v>
-      </c>
-      <c r="F27">
-        <v>1.9979843789367599E-4</v>
-      </c>
-      <c r="G27" t="s">
-        <v>27</v>
+        <v>104.583540931614</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B28">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>1.9804438276839899E-2</v>
+        <v>0.99878964906799905</v>
       </c>
       <c r="E28">
-        <v>0.103319036805502</v>
-      </c>
-      <c r="F28">
-        <v>0.21904452371515301</v>
-      </c>
-      <c r="G28" t="s">
-        <v>33</v>
+        <v>120.42979476638</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B29">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29">
-        <v>0.69166027314956002</v>
+        <v>0.99907574654042197</v>
       </c>
       <c r="E29">
-        <v>0.70215885704890402</v>
-      </c>
-      <c r="F29">
-        <v>8.3805346700083494E-2</v>
-      </c>
-      <c r="G29" t="s">
-        <v>40</v>
+        <v>192.17928496383001</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B30">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30">
-        <v>0.13288787655762699</v>
+        <v>6.8118664365912802E-3</v>
       </c>
       <c r="E30">
-        <v>0.19934149122101599</v>
+        <v>4.8283062270565403E-3</v>
       </c>
       <c r="F30">
-        <v>5.8551320830812603E-2</v>
+        <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31">
-        <v>0.114667056650596</v>
+        <v>3.5928971402492899E-3</v>
       </c>
       <c r="E31">
-        <v>8.9543392614108402E-2</v>
+        <v>9.1002532901090106E-3</v>
       </c>
       <c r="F31">
-        <v>2.3622931442080299E-2</v>
+        <v>6.2723467862481298E-3</v>
       </c>
       <c r="G31" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B32">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32">
-        <v>0.56464335766478502</v>
+        <v>9.8694983153751296E-3</v>
       </c>
       <c r="E32">
-        <v>1.44037071897738</v>
+        <v>2.3443665060524199E-2</v>
       </c>
       <c r="F32">
-        <v>3.8215125201546299E-3</v>
+        <v>2.6343263742278501E-2</v>
       </c>
       <c r="G32" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B33">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33">
-        <v>0.30062668071299098</v>
+        <v>2.11816620144437E-2</v>
       </c>
       <c r="E33">
-        <v>0.232858912244334</v>
-      </c>
-      <c r="F33" s="1">
-        <v>1.5795448936275199E-6</v>
+        <v>4.2650203333278902E-2</v>
+      </c>
+      <c r="F33">
+        <v>2.16337438355787E-3</v>
       </c>
       <c r="G33" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -4639,27 +4595,27 @@
         <v>10</v>
       </c>
       <c r="B34">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34">
-        <v>6.1991298998252398E-3</v>
+        <v>1.9804438276839899E-2</v>
       </c>
       <c r="E34">
-        <v>1.09048088947543E-2</v>
-      </c>
-      <c r="F34" s="1">
-        <v>5.4436744122842702E-5</v>
+        <v>0.103319036805502</v>
+      </c>
+      <c r="F34">
+        <v>0.21904452371515301</v>
       </c>
       <c r="G34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B35">
         <v>6</v>
@@ -4668,102 +4624,96 @@
         <v>1</v>
       </c>
       <c r="D35">
-        <v>2.7182399970635401E-2</v>
+        <v>6.1991298998252398E-3</v>
       </c>
       <c r="E35">
-        <v>2.6859700149512E-2</v>
-      </c>
-      <c r="F35">
-        <v>2.1281095020829199E-2</v>
+        <v>1.09048088947543E-2</v>
+      </c>
+      <c r="F35" s="1">
+        <v>5.4436744122842702E-5</v>
       </c>
       <c r="G35" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B36">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D36">
-        <v>4.5422534630289802E-3</v>
+        <v>-3.8509582035564601E-3</v>
       </c>
       <c r="E36">
-        <v>1.42773728656134E-2</v>
+        <v>5.4179782542063603E-3</v>
       </c>
       <c r="F36">
-        <v>4.5701787994891399E-2</v>
-      </c>
-      <c r="G36" t="s">
-        <v>48</v>
+        <v>3.73224519855059</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B37">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D37">
-        <v>7.8324879841947401E-2</v>
+        <v>1.60795515320545E-3</v>
       </c>
       <c r="E37">
-        <v>9.3641798006531093E-2</v>
+        <v>1.18150108422427E-2</v>
       </c>
       <c r="F37">
-        <v>1.09255003351527E-2</v>
-      </c>
-      <c r="G37" t="s">
-        <v>55</v>
+        <v>8.3950487952230599</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B38">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C38">
         <v>3</v>
       </c>
       <c r="D38">
-        <v>3.3551311292107799</v>
+        <v>8.8130415497322395E-3</v>
       </c>
       <c r="E38">
-        <v>1.4290055912144</v>
+        <v>3.6981726867356401E-2</v>
       </c>
       <c r="F38">
-        <v>2958.6010430657702</v>
+        <v>16.475461297818502</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B39">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C39">
         <v>3</v>
       </c>
-      <c r="D39">
-        <v>3.73604017574681</v>
-      </c>
-      <c r="E39">
-        <v>1.74830314749601</v>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
       </c>
       <c r="F39">
-        <v>2400.21863787146</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -4771,139 +4721,142 @@
         <v>10</v>
       </c>
       <c r="B40">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D40">
-        <v>-3.8509582035564601E-3</v>
+        <v>1.80962090831297E-2</v>
       </c>
       <c r="E40">
-        <v>5.4179782542063603E-3</v>
+        <v>1.02117872348011E-2</v>
       </c>
       <c r="F40">
-        <v>3.73224519855059</v>
+        <v>1.24793857861122E-2</v>
+      </c>
+      <c r="G40" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D41">
-        <v>-6.3485895354970703E-3</v>
+        <v>0.90131482045701805</v>
       </c>
       <c r="E41">
-        <v>1.1624062439954E-2</v>
-      </c>
-      <c r="F41">
-        <v>8.3539700131760792</v>
+        <v>57.836757723062597</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B42">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D42">
-        <v>5.8143075288297197E-4</v>
+        <v>0.99887864213968003</v>
       </c>
       <c r="E42">
-        <v>3.1862309406171501E-3</v>
-      </c>
-      <c r="F42">
-        <v>3.4371413213338502</v>
+        <v>103.614737619854</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B43">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D43">
-        <v>-1.1437091976826901E-2</v>
+        <v>0.99887838776928395</v>
       </c>
       <c r="E43">
-        <v>8.8433348911657692E-3</v>
-      </c>
-      <c r="F43">
-        <v>4.5735896041796096</v>
+        <v>147.642354791663</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B44">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D44">
-        <v>1.6353867628952901</v>
+        <v>1.0587518011335E-2</v>
       </c>
       <c r="E44">
-        <v>0.72960658629280795</v>
+        <v>8.2919013696786201E-3</v>
       </c>
       <c r="F44">
-        <v>11.5798418384553</v>
+        <v>2.1615585531971101E-3</v>
+      </c>
+      <c r="G44" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B45">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D45">
-        <v>1.7839608746771101</v>
+        <v>3.0550116101209099E-2</v>
       </c>
       <c r="E45">
-        <v>0.85988434003665404</v>
+        <v>4.55405009888704E-2</v>
       </c>
       <c r="F45">
-        <v>722.21443075240495</v>
+        <v>4.5264828407062E-3</v>
+      </c>
+      <c r="G45" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B46">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D46">
-        <v>1.60795515320545E-3</v>
+        <v>0.11265892621963999</v>
       </c>
       <c r="E46">
-        <v>1.18150108422427E-2</v>
+        <v>0.108580538600536</v>
       </c>
       <c r="F46">
-        <v>8.3950487952230599</v>
+        <v>1.8662441527086099E-2</v>
+      </c>
+      <c r="G46" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -4911,104 +4864,113 @@
         <v>11</v>
       </c>
       <c r="B47">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C47">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D47">
-        <v>-1.62881542550516E-2</v>
+        <v>0.23598936342653201</v>
       </c>
       <c r="E47">
-        <v>1.63680388769116E-2</v>
+        <v>0.24610894859351301</v>
       </c>
       <c r="F47">
-        <v>21.5579968111185</v>
+        <v>3.8315761234071002E-2</v>
+      </c>
+      <c r="G47" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B48">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C48">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D48">
-        <v>-1.6724522146506299E-2</v>
+        <v>0.69166027314956002</v>
       </c>
       <c r="E48">
-        <v>1.05707615765901E-2</v>
+        <v>0.70215885704890402</v>
       </c>
       <c r="F48">
-        <v>20.688538789756201</v>
+        <v>8.3805346700083494E-2</v>
+      </c>
+      <c r="G48" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B49">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C49">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D49">
-        <v>-1.27557584382472E-2</v>
+        <v>2.7182399970635401E-2</v>
       </c>
       <c r="E49">
-        <v>1.7169453163615199E-2</v>
+        <v>2.6859700149512E-2</v>
       </c>
       <c r="F49">
-        <v>13.9331043798514</v>
+        <v>2.1281095020829199E-2</v>
+      </c>
+      <c r="G49" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50">
         <v>7</v>
-      </c>
-      <c r="B50">
-        <v>9</v>
       </c>
       <c r="C50">
         <v>3</v>
       </c>
       <c r="D50">
-        <v>1.4431938998148399</v>
+        <v>-6.3485895354970703E-3</v>
       </c>
       <c r="E50">
-        <v>0.41701373301734701</v>
+        <v>1.1624062439954E-2</v>
       </c>
       <c r="F50">
-        <v>92.637575278335405</v>
+        <v>8.3539700131760792</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51">
         <v>8</v>
-      </c>
-      <c r="B51">
-        <v>9</v>
       </c>
       <c r="C51">
         <v>3</v>
       </c>
-      <c r="D51" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" t="s">
-        <v>9</v>
+      <c r="D51">
+        <v>-1.62881542550516E-2</v>
+      </c>
+      <c r="E51">
+        <v>1.63680388769116E-2</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <v>21.5579968111185</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B52">
         <v>9</v>
@@ -5017,13 +4979,13 @@
         <v>3</v>
       </c>
       <c r="D52">
-        <v>8.8130415497322395E-3</v>
+        <v>1.7864574667319999E-2</v>
       </c>
       <c r="E52">
-        <v>3.6981726867356401E-2</v>
+        <v>5.3308140919319201E-2</v>
       </c>
       <c r="F52">
-        <v>16.475461297818502</v>
+        <v>17.274856208580299</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -5031,139 +4993,139 @@
         <v>11</v>
       </c>
       <c r="B53">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C53">
         <v>3</v>
       </c>
       <c r="D53">
-        <v>1.7864574667319999E-2</v>
+        <v>-7.1265219976306199E-3</v>
       </c>
       <c r="E53">
-        <v>5.3308140919319201E-2</v>
+        <v>4.6026459290012998E-2</v>
       </c>
       <c r="F53">
-        <v>17.274856208580299</v>
+        <v>20.532268011398301</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B54">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C54">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D54">
-        <v>1.28091898596541E-2</v>
+        <v>4.1534307380159001E-2</v>
       </c>
       <c r="E54">
-        <v>4.8782212736154497E-2</v>
+        <v>0.18578490323079699</v>
       </c>
       <c r="F54">
-        <v>8.8928416489703999</v>
+        <v>0.10108020895325</v>
+      </c>
+      <c r="G54" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B55">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D55">
-        <v>1.7205518099969101E-3</v>
+        <v>0.99467285970653396</v>
       </c>
       <c r="E55">
-        <v>2.77174968895409E-2</v>
-      </c>
-      <c r="F55">
-        <v>14.220309217000301</v>
+        <v>61.460421126414303</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B56">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C56">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D56">
-        <v>1.56569575936312</v>
+        <v>0.99230566953452404</v>
       </c>
       <c r="E56">
-        <v>0.63742375503896198</v>
-      </c>
-      <c r="F56">
-        <v>2604.4148449139602</v>
+        <v>102.898713434359</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B57">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C57">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D57">
-        <v>1.7787607912916501</v>
+        <v>0.99673290485723298</v>
       </c>
       <c r="E57">
-        <v>0.89380641613968603</v>
-      </c>
-      <c r="F57">
-        <v>9.3435874212267596</v>
+        <v>122.30985296421601</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B58">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>3</v>
-      </c>
-      <c r="D58" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>1.6435212053167499E-2</v>
+      </c>
+      <c r="E58">
+        <v>7.1600894317287202E-3</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>7.5788442548485203E-3</v>
+      </c>
+      <c r="G58" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B59">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C59">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D59">
-        <v>-7.1265219976306199E-3</v>
+        <v>3.6438361299231401E-3</v>
       </c>
       <c r="E59">
-        <v>4.6026459290012998E-2</v>
+        <v>2.2271907976498199E-2</v>
       </c>
       <c r="F59">
-        <v>20.532268011398301</v>
+        <v>5.79054916985951E-3</v>
+      </c>
+      <c r="G59" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -5171,131 +5133,131 @@
         <v>12</v>
       </c>
       <c r="B60">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C60">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D60">
-        <v>-1.5287669224566799E-2</v>
+        <v>3.15363396795416E-2</v>
       </c>
       <c r="E60">
-        <v>1.3265963523E-2</v>
+        <v>4.67932663299108E-2</v>
       </c>
       <c r="F60">
-        <v>18.168263855387</v>
+        <v>4.5415234822451297E-3</v>
+      </c>
+      <c r="G60" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B61">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C61">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D61">
-        <v>2.0956040649207301E-4</v>
+        <v>7.9863795705357205E-2</v>
       </c>
       <c r="E61">
-        <v>3.5804244139803397E-2</v>
+        <v>8.7966792709945105E-2</v>
       </c>
       <c r="F61">
-        <v>17.192286249248301</v>
+        <v>1.12795535261288E-2</v>
+      </c>
+      <c r="G61" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B62">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62">
-        <v>1.31005315718724</v>
+        <v>0.13288787655762699</v>
       </c>
       <c r="E62">
-        <v>1.2056962269094</v>
-      </c>
-      <c r="F62" s="1">
-        <v>4.8176855683120603E-6</v>
+        <v>0.19934149122101599</v>
+      </c>
+      <c r="F62">
+        <v>5.8551320830812603E-2</v>
       </c>
       <c r="G62" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B63">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63">
-        <v>0.62275282626455197</v>
+        <v>4.5422534630289802E-3</v>
       </c>
       <c r="E63">
-        <v>0.89833380224297898</v>
+        <v>1.42773728656134E-2</v>
       </c>
       <c r="F63">
-        <v>2.3133224739621898E-3</v>
+        <v>4.5701787994891399E-2</v>
       </c>
       <c r="G63" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B64">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D64">
-        <v>1.80962090831297E-2</v>
+        <v>5.8143075288297197E-4</v>
       </c>
       <c r="E64">
-        <v>1.02117872348011E-2</v>
+        <v>3.1862309406171501E-3</v>
       </c>
       <c r="F64">
-        <v>1.24793857861122E-2</v>
-      </c>
-      <c r="G64" t="s">
-        <v>28</v>
+        <v>3.4371413213338502</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B65">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D65">
-        <v>4.1534307380159001E-2</v>
+        <v>-1.6724522146506299E-2</v>
       </c>
       <c r="E65">
-        <v>0.18578490323079699</v>
+        <v>1.05707615765901E-2</v>
       </c>
       <c r="F65">
-        <v>0.10108020895325</v>
-      </c>
-      <c r="G65" t="s">
-        <v>35</v>
+        <v>20.688538789756201</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -5303,67 +5265,67 @@
         <v>12</v>
       </c>
       <c r="B66">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D66">
-        <v>0.295913985781037</v>
+        <v>1.28091898596541E-2</v>
       </c>
       <c r="E66">
-        <v>0.71980425151465199</v>
+        <v>4.8782212736154497E-2</v>
       </c>
       <c r="F66">
-        <v>0.116538569604086</v>
-      </c>
-      <c r="G66" t="s">
-        <v>42</v>
+        <v>8.8928416489703999</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B67">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D67">
-        <v>8.4025692400866395E-2</v>
+        <v>-1.5287669224566799E-2</v>
       </c>
       <c r="E67">
-        <v>7.1780358383399606E-2</v>
+        <v>1.3265963523E-2</v>
       </c>
       <c r="F67">
-        <v>0.14097088959111301</v>
-      </c>
-      <c r="G67" t="s">
-        <v>50</v>
+        <v>18.168263855387</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B68">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D68">
-        <v>0.99978597990104101</v>
+        <v>0.295913985781037</v>
       </c>
       <c r="E68">
-        <v>572.24332754043496</v>
+        <v>0.71980425151465199</v>
+      </c>
+      <c r="F68">
+        <v>0.116538569604086</v>
+      </c>
+      <c r="G68" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B69">
         <v>12</v>
@@ -5372,61 +5334,67 @@
         <v>2</v>
       </c>
       <c r="D69">
-        <v>0.99999974794416902</v>
+        <v>0.99419111917237601</v>
       </c>
       <c r="E69">
-        <v>104.583540931614</v>
+        <v>52.808222927565602</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B70">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C70">
         <v>2</v>
       </c>
       <c r="D70">
-        <v>0.90131482045701805</v>
+        <v>0.99250232989647202</v>
       </c>
       <c r="E70">
-        <v>57.836757723062597</v>
+        <v>95.226853289546</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B71">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C71">
         <v>2</v>
       </c>
       <c r="D71">
-        <v>0.99467285970653396</v>
+        <v>0.98742092651757196</v>
       </c>
       <c r="E71">
-        <v>61.460421126414303</v>
+        <v>140.324494817226</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B72">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D72">
-        <v>0.99419111917237601</v>
+        <v>1.7977434108671801E-2</v>
       </c>
       <c r="E72">
-        <v>52.808222927565602</v>
+        <v>1.8647753703395401E-2</v>
+      </c>
+      <c r="F72">
+        <v>1.5082738977944101E-3</v>
+      </c>
+      <c r="G72" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -5434,101 +5402,134 @@
         <v>13</v>
       </c>
       <c r="B73">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D73">
-        <v>0.99999848507801803</v>
+        <v>2.7812285502499499E-2</v>
       </c>
       <c r="E73">
-        <v>49.373286109629603</v>
+        <v>1.9913199960123799E-2</v>
+      </c>
+      <c r="F73" s="1">
+        <v>8.61821315713875E-7</v>
+      </c>
+      <c r="G73" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B74">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D74">
-        <v>0.99958593898769799</v>
+        <v>2.6055156398218999E-2</v>
       </c>
       <c r="E74">
-        <v>710.31946600416597</v>
+        <v>2.4400456291021701E-2</v>
+      </c>
+      <c r="F74">
+        <v>1.1706156009953399E-3</v>
+      </c>
+      <c r="G74" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B75">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D75">
-        <v>0.99878964906799905</v>
+        <v>1.5277419708914599E-2</v>
       </c>
       <c r="E75">
-        <v>120.42979476638</v>
+        <v>4.8098007247903099E-2</v>
+      </c>
+      <c r="F75">
+        <v>1.6403662575491899E-4</v>
+      </c>
+      <c r="G75" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B76">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D76">
-        <v>0.99887864213968003</v>
+        <v>0.114667056650596</v>
       </c>
       <c r="E76">
-        <v>103.614737619854</v>
+        <v>8.9543392614108402E-2</v>
+      </c>
+      <c r="F76">
+        <v>2.3622931442080299E-2</v>
+      </c>
+      <c r="G76" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B77">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C77">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D77">
-        <v>0.99230566953452404</v>
+        <v>7.8324879841947401E-2</v>
       </c>
       <c r="E77">
-        <v>102.898713434359</v>
+        <v>9.3641798006531093E-2</v>
+      </c>
+      <c r="F77">
+        <v>1.09255003351527E-2</v>
+      </c>
+      <c r="G77" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B78">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C78">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D78">
-        <v>0.99250232989647202</v>
+        <v>-1.1437091976826901E-2</v>
       </c>
       <c r="E78">
-        <v>95.226853289546</v>
+        <v>8.8433348911657692E-3</v>
+      </c>
+      <c r="F78">
+        <v>4.5735896041796096</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -5536,104 +5537,119 @@
         <v>13</v>
       </c>
       <c r="B79">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C79">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D79">
-        <v>0.99999861569922899</v>
+        <v>-1.27557584382472E-2</v>
       </c>
       <c r="E79">
-        <v>82.672079717461898</v>
+        <v>1.7169453163615199E-2</v>
+      </c>
+      <c r="F79">
+        <v>13.9331043798514</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B80">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C80">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D80">
-        <v>0.99999944308530697</v>
+        <v>1.7205518099969101E-3</v>
       </c>
       <c r="E80">
-        <v>145.938586744144</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.77174968895409E-2</v>
+      </c>
+      <c r="F80">
+        <v>14.220309217000301</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B81">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C81">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D81">
-        <v>0.99907574654042197</v>
+        <v>2.0956040649207301E-4</v>
       </c>
       <c r="E81">
-        <v>192.17928496383001</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.5804244139803397E-2</v>
+      </c>
+      <c r="F81">
+        <v>17.192286249248301</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B82">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D82">
-        <v>0.99887838776928395</v>
+        <v>8.4025692400866395E-2</v>
       </c>
       <c r="E82">
-        <v>147.642354791663</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7.1780358383399606E-2</v>
+      </c>
+      <c r="F82">
+        <v>0.14097088959111301</v>
+      </c>
+      <c r="G82" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B83">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C83">
         <v>2</v>
       </c>
       <c r="D83">
-        <v>0.99673290485723298</v>
+        <v>0.99999848507801803</v>
       </c>
       <c r="E83">
-        <v>122.30985296421601</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49.373286109629603</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B84">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C84">
         <v>2</v>
       </c>
       <c r="D84">
-        <v>0.98742092651757196</v>
+        <v>0.99999861569922899</v>
       </c>
       <c r="E84">
-        <v>140.324494817226</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+        <v>82.672079717461898</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>13</v>
       </c>
@@ -5651,9 +5667,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G85">
-    <sortState ref="A2:G85">
-      <sortCondition ref="B1:B85"/>
+  <autoFilter ref="A1:G85" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G85">
+      <sortCondition ref="A1:A85"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5661,14 +5677,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" activeCellId="1" sqref="A1:C1048576 F1:F1048576"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -5745,7 +5761,7 @@
         <v>0.49755684</v>
       </c>
       <c r="K2">
-        <f>GEOMEAN(G2:J2)</f>
+        <f t="shared" ref="K2:K31" si="0">GEOMEAN(G2:J2)</f>
         <v>0.85390724061935408</v>
       </c>
     </row>
@@ -5781,7 +5797,7 @@
         <v>1.47468848</v>
       </c>
       <c r="K3">
-        <f>GEOMEAN(G3:J3)</f>
+        <f t="shared" si="0"/>
         <v>2.8836192060410113</v>
       </c>
     </row>
@@ -5817,7 +5833,7 @@
         <v>4.1820682700000003</v>
       </c>
       <c r="K4">
-        <f>GEOMEAN(G4:J4)</f>
+        <f t="shared" si="0"/>
         <v>4.4883181333727498</v>
       </c>
     </row>
@@ -5853,7 +5869,7 @@
         <v>4.08184228</v>
       </c>
       <c r="K5">
-        <f>GEOMEAN(G5:J5)</f>
+        <f t="shared" si="0"/>
         <v>3.9198256861618006</v>
       </c>
     </row>
@@ -5889,7 +5905,7 @@
         <v>2.9717724599999999</v>
       </c>
       <c r="K6">
-        <f>GEOMEAN(G6:J6)</f>
+        <f t="shared" si="0"/>
         <v>4.7792446950252314</v>
       </c>
     </row>
@@ -5925,7 +5941,7 @@
         <v>0.27182823</v>
       </c>
       <c r="K7">
-        <f>GEOMEAN(G7:J7)</f>
+        <f t="shared" si="0"/>
         <v>0.84826134111892326</v>
       </c>
     </row>
@@ -5961,7 +5977,7 @@
         <v>2.4891932200000002</v>
       </c>
       <c r="K8">
-        <f>GEOMEAN(G8:J8)</f>
+        <f t="shared" si="0"/>
         <v>2.8347539121128857</v>
       </c>
     </row>
@@ -5997,7 +6013,7 @@
         <v>3.6085126999999999</v>
       </c>
       <c r="K9">
-        <f>GEOMEAN(G9:J9)</f>
+        <f t="shared" si="0"/>
         <v>4.8120369829317182</v>
       </c>
     </row>
@@ -6033,7 +6049,7 @@
         <v>2.9661827999999999</v>
       </c>
       <c r="K10">
-        <f>GEOMEAN(G10:J10)</f>
+        <f t="shared" si="0"/>
         <v>4.1715342354244447</v>
       </c>
     </row>
@@ -6069,7 +6085,7 @@
         <v>2.80174594</v>
       </c>
       <c r="K11">
-        <f>GEOMEAN(G11:J11)</f>
+        <f t="shared" si="0"/>
         <v>4.8569285720067672</v>
       </c>
     </row>
@@ -6105,7 +6121,7 @@
         <v>2.80443628</v>
       </c>
       <c r="K12">
-        <f>GEOMEAN(G12:J12)</f>
+        <f t="shared" si="0"/>
         <v>2.0188386986403311</v>
       </c>
     </row>
@@ -6141,7 +6157,7 @@
         <v>1.8324411700000001</v>
       </c>
       <c r="K13">
-        <f>GEOMEAN(G13:J13)</f>
+        <f t="shared" si="0"/>
         <v>2.1520254800682355</v>
       </c>
     </row>
@@ -6177,7 +6193,7 @@
         <v>1.8758246700000001</v>
       </c>
       <c r="K14">
-        <f>GEOMEAN(G14:J14)</f>
+        <f t="shared" si="0"/>
         <v>2.9807469075273367</v>
       </c>
     </row>
@@ -6213,7 +6229,7 @@
         <v>4.2210377299999999</v>
       </c>
       <c r="K15">
-        <f>GEOMEAN(G15:J15)</f>
+        <f t="shared" si="0"/>
         <v>4.0649665260390853</v>
       </c>
     </row>
@@ -6249,7 +6265,7 @@
         <v>2.3742615200000001</v>
       </c>
       <c r="K16">
-        <f>GEOMEAN(G16:J16)</f>
+        <f t="shared" si="0"/>
         <v>2.9756362374291125</v>
       </c>
     </row>
@@ -6285,7 +6301,7 @@
         <v>2.5484705700000001</v>
       </c>
       <c r="K17">
-        <f>GEOMEAN(G17:J17)</f>
+        <f t="shared" si="0"/>
         <v>1.0370241183765418</v>
       </c>
     </row>
@@ -6321,7 +6337,7 @@
         <v>2.8462189200000001</v>
       </c>
       <c r="K18">
-        <f>GEOMEAN(G18:J18)</f>
+        <f t="shared" si="0"/>
         <v>3.8390095194311136</v>
       </c>
     </row>
@@ -6357,7 +6373,7 @@
         <v>3.3860594800000001</v>
       </c>
       <c r="K19">
-        <f>GEOMEAN(G19:J19)</f>
+        <f t="shared" si="0"/>
         <v>3.7480346451513888</v>
       </c>
     </row>
@@ -6393,7 +6409,7 @@
         <v>2.99012514</v>
       </c>
       <c r="K20">
-        <f>GEOMEAN(G20:J20)</f>
+        <f t="shared" si="0"/>
         <v>3.6785276046942017</v>
       </c>
     </row>
@@ -6429,7 +6445,7 @@
         <v>2.6259252000000002</v>
       </c>
       <c r="K21">
-        <f>GEOMEAN(G21:J21)</f>
+        <f t="shared" si="0"/>
         <v>3.499509714224271</v>
       </c>
     </row>
@@ -6465,7 +6481,7 @@
         <v>1.87772899</v>
       </c>
       <c r="K22">
-        <f>GEOMEAN(G22:J22)</f>
+        <f t="shared" si="0"/>
         <v>1.7343675235830989</v>
       </c>
     </row>
@@ -6501,7 +6517,7 @@
         <v>2.8999232799999999</v>
       </c>
       <c r="K23">
-        <f>GEOMEAN(G23:J23)</f>
+        <f t="shared" si="0"/>
         <v>3.4114064694524031</v>
       </c>
     </row>
@@ -6537,7 +6553,7 @@
         <v>3.8006742</v>
       </c>
       <c r="K24">
-        <f>GEOMEAN(G24:J24)</f>
+        <f t="shared" si="0"/>
         <v>3.8804606988070414</v>
       </c>
     </row>
@@ -6573,7 +6589,7 @@
         <v>3.7121535699999999</v>
       </c>
       <c r="K25">
-        <f>GEOMEAN(G25:J25)</f>
+        <f t="shared" si="0"/>
         <v>3.6545757007621482</v>
       </c>
     </row>
@@ -6609,7 +6625,7 @@
         <v>3.3361942500000001</v>
       </c>
       <c r="K26">
-        <f>GEOMEAN(G26:J26)</f>
+        <f t="shared" si="0"/>
         <v>3.7096878363526624</v>
       </c>
     </row>
@@ -6645,7 +6661,7 @@
         <v>1.7637902299999999</v>
       </c>
       <c r="K27">
-        <f>GEOMEAN(G27:J27)</f>
+        <f t="shared" si="0"/>
         <v>2.1570358279783814</v>
       </c>
     </row>
@@ -6681,7 +6697,7 @@
         <v>3.1018012700000002</v>
       </c>
       <c r="K28">
-        <f>GEOMEAN(G28:J28)</f>
+        <f t="shared" si="0"/>
         <v>4.1956934447431404</v>
       </c>
     </row>
@@ -6717,7 +6733,7 @@
         <v>3.5591479700000002</v>
       </c>
       <c r="K29">
-        <f>GEOMEAN(G29:J29)</f>
+        <f t="shared" si="0"/>
         <v>4.4229696432734951</v>
       </c>
     </row>
@@ -6753,7 +6769,7 @@
         <v>3.47755467</v>
       </c>
       <c r="K30">
-        <f>GEOMEAN(G30:J30)</f>
+        <f t="shared" si="0"/>
         <v>4.125574346005684</v>
       </c>
     </row>
@@ -6789,13 +6805,13 @@
         <v>2.96831859</v>
       </c>
       <c r="K31">
-        <f>GEOMEAN(G31:J31)</f>
+        <f t="shared" si="0"/>
         <v>4.4839532074437001</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K31">
-    <sortState ref="A2:K31">
+  <autoFilter ref="A1:K31" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K31">
       <sortCondition ref="A1:A31"/>
     </sortState>
   </autoFilter>
@@ -6804,14 +6820,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -6963,14 +6979,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -7122,14 +7138,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>